<commit_message>
Units / Attributes  - Generating change value factors for armor and damage
</commit_message>
<xml_diff>
--- a/DisciplesBattleSimulator/src/units/data/Wspolczynniki_zmiany.xlsx
+++ b/DisciplesBattleSimulator/src/units/data/Wspolczynniki_zmiany.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="25875" windowHeight="8760"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="25875" windowHeight="8760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Spadek obrażeń" sheetId="1" r:id="rId1"/>
+    <sheet name="Spadek pancerza" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,13 +16,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Ochrona</t>
+  </si>
+  <si>
+    <t>Spadek</t>
+  </si>
+  <si>
+    <t>Życie</t>
+  </si>
+  <si>
+    <t>&gt; 90</t>
+  </si>
+  <si>
+    <t>&gt; 1200</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -50,9 +81,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D40"/>
+  <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -366,469 +404,474 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>70</v>
-      </c>
-      <c r="C2">
-        <f>1*(1-(0.025*A2))</f>
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <f>1-(0.025*A3)</f>
         <v>1</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C40" si="0">1*(1-(0.025*A3))</f>
-        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.95</v>
+        <f t="shared" ref="C4:C41" si="0">1-(0.025*A4)</f>
+        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.92500000000000004</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.82499999999999996</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>340</v>
+        <v>310</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.77500000000000002</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>370</v>
+        <v>340</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>400</v>
+        <v>370</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.72499999999999998</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>460</v>
+        <v>430</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.67500000000000004</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>490</v>
+        <v>460</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.64999999999999991</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>520</v>
+        <v>490</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.64999999999999991</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>580</v>
+        <v>550</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.57499999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>610</v>
+        <v>580</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>640</v>
+        <v>610</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0.52499999999999991</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>670</v>
+        <v>640</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.52499999999999991</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>700</v>
+        <v>670</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0.47499999999999998</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>730</v>
+        <v>700</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
+        <v>0.47499999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>760</v>
+        <v>730</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>0.42499999999999993</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>790</v>
+        <v>760</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>0.39999999999999991</v>
+        <v>0.42499999999999993</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>820</v>
+        <v>790</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.39999999999999991</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
-        <v>850</v>
+        <v>820</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>880</v>
+        <v>850</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>0.32499999999999996</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>910</v>
+        <v>880</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>0.29999999999999993</v>
+        <v>0.32499999999999996</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31">
-        <v>940</v>
+        <v>910</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>0.27499999999999991</v>
+        <v>0.29999999999999993</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>970</v>
+        <v>940</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.27499999999999991</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>1000</v>
+        <v>970</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>0.22499999999999998</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34">
-        <v>1030</v>
+        <v>1000</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>0.19999999999999996</v>
+        <v>0.22499999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35">
-        <v>1060</v>
+        <v>1030</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>0.17499999999999993</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36">
-        <v>1090</v>
+        <v>1060</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>0.14999999999999991</v>
+        <v>0.17499999999999993</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37">
-        <v>1120</v>
+        <v>1090</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.14999999999999991</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38">
-        <v>1150</v>
+        <v>1120</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
-        <v>1180</v>
+        <v>1150</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>7.4999999999999956E-2</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>1180</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999956E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>1210</v>
-      </c>
-      <c r="C40">
+      <c r="B41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41">
         <f t="shared" si="0"/>
         <v>4.9999999999999933E-2</v>
       </c>
@@ -841,13 +884,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f>(100-B3)/100</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C21" si="0">(100-B4)/100</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>65</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>75</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>85</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>